<commit_message>
ProjectCreation.java and Name test work properly
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ProjectCreation.xlsx
+++ b/scrummetrics/excel/ProjectCreation.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD86AC7-0D92-4439-B592-276FA25C86BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42B09DC-E760-45E9-9CE4-139BDF1D57D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
-    <sheet name="Existing" sheetId="1" r:id="rId1"/>
+    <sheet name="Mandatory name" sheetId="1" r:id="rId1"/>
     <sheet name="Non existing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -37,13 +37,40 @@
     <t>P4ssword.</t>
   </si>
   <si>
-    <t>jositom</t>
-  </si>
-  <si>
     <t>asdfuser</t>
   </si>
   <si>
     <t>qweruser</t>
+  </si>
+  <si>
+    <t>angel_dlr</t>
+  </si>
+  <si>
+    <t>Pa$$w0rd</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>Testing Project</t>
+  </si>
+  <si>
+    <t>During this project we expect on having successful tests that will prove that our software works properly.</t>
+  </si>
+  <si>
+    <t>18 October 2021</t>
+  </si>
+  <si>
+    <t>Create optimal test cases to perform for the correct operation of the program</t>
+  </si>
+  <si>
+    <t>15 October 2021</t>
   </si>
 </sst>
 </file>
@@ -421,10 +448,14 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -433,21 +464,45 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -486,7 +541,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -494,7 +549,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>

</xml_diff>